<commit_message>
Adding TestRun Manager file
</commit_message>
<xml_diff>
--- a/Testing/resources/TestRunManager.xlsx
+++ b/Testing/resources/TestRunManager.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Test Case 1</t>
   </si>
@@ -29,6 +29,15 @@
   </si>
   <si>
     <t>YES</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>TestStartTime</t>
+  </si>
+  <si>
+    <t>TestEndTime</t>
   </si>
 </sst>
 </file>
@@ -399,11 +408,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="F9" sqref="F9"/>
+      <selection pane="topRight" activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -411,10 +420,13 @@
     <col min="1" max="1" width="7.5703125" style="4" customWidth="1"/>
     <col min="2" max="2" width="58.85546875" style="4" customWidth="1"/>
     <col min="3" max="3" width="34.140625" style="4" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="3"/>
+    <col min="4" max="4" width="9.140625" style="3"/>
+    <col min="5" max="5" width="13.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -424,8 +436,17 @@
       <c r="C1" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:6">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -443,6 +464,5 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>